<commit_message>
Update Data Analyst project tracker.xlsx
</commit_message>
<xml_diff>
--- a/Data Analyst project tracker.xlsx
+++ b/Data Analyst project tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\1st_data_analysis\1st-data-analysis-project git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F80A0FE-A0E3-41DA-86C3-DDAE0904BDF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348D63A6-6585-4FCF-A5F4-A510A2BC1E4F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
   <si>
     <t>SL #</t>
   </si>
@@ -133,6 +133,21 @@
   </si>
   <si>
     <t>Excected and learnt analytical functions like rank, desc_rank, with. Downloaded github and Uploaded the 1st data set analysis to github.</t>
+  </si>
+  <si>
+    <t>completed</t>
+  </si>
+  <si>
+    <t>4hr</t>
+  </si>
+  <si>
+    <t>Learned powerBi tool and pull the excel sheet dataset to the powerBI</t>
+  </si>
+  <si>
+    <t>manually build the E-R diagram and relatioship between the tables</t>
+  </si>
+  <si>
+    <t>understood different graph and explored tooltip, drill down</t>
   </si>
 </sst>
 </file>
@@ -182,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -199,12 +214,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -524,7 +542,7 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,7 +552,7 @@
     <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" customWidth="1"/>
-    <col min="7" max="7" width="61.5703125" customWidth="1"/>
+    <col min="7" max="7" width="66.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -579,7 +597,7 @@
       <c r="F2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>30</v>
       </c>
     </row>
@@ -587,7 +605,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
@@ -602,7 +620,7 @@
       <c r="F3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="7" t="s">
         <v>31</v>
       </c>
     </row>
@@ -610,7 +628,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="10"/>
       <c r="C4" t="s">
         <v>9</v>
       </c>
@@ -623,7 +641,7 @@
       <c r="F4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>34</v>
       </c>
     </row>
@@ -631,7 +649,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C5" t="s">
@@ -646,7 +664,7 @@
       <c r="F5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>33</v>
       </c>
     </row>
@@ -654,7 +672,7 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="10"/>
       <c r="C6" t="s">
         <v>11</v>
       </c>
@@ -667,7 +685,7 @@
       <c r="F6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="7" t="s">
         <v>32</v>
       </c>
     </row>
@@ -675,11 +693,11 @@
       <c r="A7">
         <v>7</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <v>44301</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -688,44 +706,80 @@
       <c r="F7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
+      </c>
+      <c r="D8" s="2">
+        <v>44305</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="10"/>
       <c r="C9" t="s">
         <v>14</v>
+      </c>
+      <c r="D9" s="2">
+        <v>44308</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="10"/>
       <c r="C10" t="s">
         <v>15</v>
+      </c>
+      <c r="D10" s="2">
+        <v>44313</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C11" t="s">
@@ -736,7 +790,7 @@
       <c r="A12">
         <v>12</v>
       </c>
-      <c r="B12" s="4"/>
+      <c r="B12" s="10"/>
       <c r="C12" t="s">
         <v>21</v>
       </c>
@@ -745,7 +799,7 @@
       <c r="A13">
         <v>13</v>
       </c>
-      <c r="B13" s="4"/>
+      <c r="B13" s="10"/>
       <c r="C13" t="s">
         <v>18</v>
       </c>
@@ -754,17 +808,17 @@
       <c r="A14">
         <v>14</v>
       </c>
-      <c r="B14" s="4"/>
+      <c r="B14" s="10"/>
       <c r="C14" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="7"/>
+      <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
-      <c r="G15" s="7"/>
+      <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -780,13 +834,13 @@
       <c r="A18">
         <v>18</v>
       </c>
-      <c r="G18" s="7"/>
+      <c r="G18" s="9"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>19</v>
       </c>
-      <c r="G19" s="7"/>
+      <c r="G19" s="9"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">

</xml_diff>